<commit_message>
This is the Excel for Model performance
</commit_message>
<xml_diff>
--- a/model_performance.xlsx
+++ b/model_performance.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Accuracy" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Classification Report" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Confusion Matrix" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Classification Report" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ROC Curve" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,25 +436,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Score</t>
+          <t>precision</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>recall</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>f1-score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>support</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Accuracy</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9801864801864801</v>
+        <v>0.8853754940711462</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9911504424778761</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9352818371607515</v>
+      </c>
+      <c r="E2" t="n">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.9886363636363636</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.9182058047493403</v>
+      </c>
+      <c r="E3" t="n">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9277389277389277</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.9277389277389277</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9277389277389277</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9277389277389277</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>macro avg</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.9370059288537549</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.9241466498103665</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9267438209550459</v>
+      </c>
+      <c r="E5" t="n">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>weighted avg</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9342378635856897</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.9277389277389277</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.9272015700756315</v>
+      </c>
+      <c r="E6" t="n">
+        <v>858</v>
       </c>
     </row>
   </sheetData>
@@ -479,39 +574,39 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pred_0</t>
+          <t>Predicted Negative</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Pred_1</t>
+          <t>Predicted Positive</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>True_0</t>
+          <t>Actual Negative</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>True_1</t>
+          <t>Actual Positive</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C3" t="n">
-        <v>403</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,118 +631,1056 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>precision</t>
+          <t>False Positive Rate</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>recall</t>
+          <t>True Positive Rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>f1-score</t>
+          <t>Threshold</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
-          <t>support</t>
+          <t>inf</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.9931972789115646</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.9690265486725663</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.9809630459126539</v>
-      </c>
-      <c r="E2" t="n">
-        <v>452</v>
-      </c>
-    </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9664268585131894</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
+        <v>0.002463054187192118</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.9998173117637634</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.01970443349753695</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.999718964099884</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0270935960591133</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9997157454490662</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.06403940886699508</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.9996271133422852</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.06896551724137931</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.9996199607849121</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7266009852216748</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9858706593513489</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.002212389380530973</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.7266009852216748</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9857752323150635</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.002212389380530973</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8004926108374384</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.8057669997215271</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.004424778761061947</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8004926108374384</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.7889406085014343</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.004424778761061947</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8399014778325123</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.6237540245056152</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.00663716814159292</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8399014778325123</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.6236355900764465</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.00663716814159292</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.854679802955665</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5158156752586365</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.008849557522123894</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.854679802955665</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5038375854492188</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.008849557522123894</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8620689655172413</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.459390789270401</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.01106194690265487</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8620689655172413</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.4258958399295807</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.01106194690265487</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8645320197044335</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.4225326478481293</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.01327433628318584</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8645320197044335</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.4064393639564514</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01327433628318584</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.8719211822660099</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.3807186186313629</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.01548672566371681</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.8719211822660099</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.3782868683338165</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.01548672566371681</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.8768472906403941</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.3533491790294647</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01769911504424779</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.8768472906403941</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.351245254278183</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.01769911504424779</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.8817733990147784</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.3371258974075317</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.01991150442477876</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.8817733990147784</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.3340949416160583</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.01991150442477876</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.8866995073891626</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.3055359125137329</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.02212389380530973</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.8866995073891626</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.2880258858203888</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.02212389380530973</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.8891625615763546</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.2766042351722717</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.02433628318584071</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.8891625615763546</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.268317699432373</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.02433628318584071</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.9039408866995073</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.2084478437900543</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.02654867256637168</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.9039408866995073</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.2066945284605026</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.02654867256637168</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.9113300492610837</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.1847250908613205</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.0331858407079646</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.9113300492610837</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.1695386916399002</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.0331858407079646</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.916256157635468</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.1467279195785522</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.0420353982300885</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.916256157635468</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.1180398911237717</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.0420353982300885</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.9261083743842364</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.1014461070299149</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.04867256637168142</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.9261083743842364</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.09915177524089813</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.04867256637168142</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.09767218679189682</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.05088495575221239</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.09390752017498016</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.05088495575221239</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.9359605911330049</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.08340216428041458</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.05530973451327434</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.9359605911330049</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.08167707175016403</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.05530973451327434</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.9384236453201971</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.07907600700855255</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.05752212389380531</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.9384236453201971</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.07679986953735352</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.05752212389380531</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.9433497536945813</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.07236941158771515</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.05973451327433629</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.9433497536945813</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.07018384337425232</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.05973451327433629</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.9482758620689655</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.06744382530450821</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.06194690265486726</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.9482758620689655</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.06633882969617844</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.06194690265486726</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.9507389162561576</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.06616678088903427</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.06415929203539823</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.9507389162561576</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.06508972495794296</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.06415929203539823</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.9532019704433498</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.06256770342588425</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.06637168141592921</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.9532019704433498</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.06178577244281769</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.06637168141592921</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.9556650246305419</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0610358864068985</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.06858407079646017</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.9556650246305419</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.06072599440813065</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.06858407079646017</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.9630541871921182</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.05927775055170059</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.08185840707964602</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.9630541871921182</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.05474657937884331</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.08185840707964602</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.9704433497536946</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.04973853752017021</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.09513274336283185</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.9704433497536946</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.04379822313785553</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.09513274336283185</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.9729064039408867</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.04290182515978813</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.1017699115044248</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.9729064039408867</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.03846105188131332</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.1017699115044248</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.9802955665024631</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.03416674211621284</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.1128318584070796</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.9802955665024631</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.03302702307701111</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.1128318584070796</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.9827586206896551</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.03238726034760475</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.1238938053097345</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.9827586206896551</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.02917665615677834</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.1238938053097345</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.9876847290640394</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0258934274315834</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.1283185840707965</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.9876847290640394</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.02479944005608559</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.1283185840707965</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.9901477832512315</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.02386130392551422</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.1327433628318584</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.9901477832512315</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.02261484041810036</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.1327433628318584</v>
+      </c>
+      <c r="C68" t="n">
         <v>0.9926108374384236</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.9793438639125152</v>
-      </c>
-      <c r="E3" t="n">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.9801864801864801</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.9801864801864801</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.9801864801864801</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.9801864801864801</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>macro avg</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.979812068712377</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.980818693055495</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.9801534549125845</v>
-      </c>
-      <c r="E5" t="n">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>weighted avg</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.9805296907044081</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.9801864801864801</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.980196859558276</v>
-      </c>
-      <c r="E6" t="n">
-        <v>858</v>
+      <c r="D68" t="n">
+        <v>0.02165526710450649</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.1438053097345133</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.9926108374384236</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.01874139904975891</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.1438053097345133</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.9950738916256158</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.01859548501670361</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.1482300884955752</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.9950738916256158</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.01824799366295338</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.1482300884955752</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.9975369458128078</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.01800906471908092</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.2986725663716814</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.9975369458128078</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.004369649104773998</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.2986725663716814</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.004236625507473946</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0001220618723891675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>